<commit_message>
Edited excel and csv files
</commit_message>
<xml_diff>
--- a/assignment2/data/vaccination_edited.xlsx
+++ b/assignment2/data/vaccination_edited.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khash\Documents\GitHub\FIT3179\assignment2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{972F47D5-C6C9-49DB-BFB8-53BEBC682080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{9CFAEE1F-7794-4AE3-8DDF-3903C2D7255C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Vaccination" sheetId="1" r:id="rId1"/>
+    <sheet name="vaccination_edited" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,18 +33,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="54">
   <si>
     <t>date</t>
-  </si>
-  <si>
-    <t>dose1_perlis</t>
-  </si>
-  <si>
-    <t>dose2_perlis</t>
-  </si>
-  <si>
-    <t>dose1_kedah</t>
   </si>
   <si>
     <t>dose2_kedah</t>
@@ -191,64 +182,19 @@
     <t>03/31/2021</t>
   </si>
   <si>
-    <t>Vaccinations</t>
-  </si>
-  <si>
     <t>Population</t>
-  </si>
-  <si>
-    <t>Nominalised vaccinations</t>
   </si>
   <si>
     <t>State</t>
   </si>
   <si>
-    <t>perlis</t>
+    <t>Dose</t>
   </si>
   <si>
-    <t>kedah</t>
+    <t>Perlis</t>
   </si>
   <si>
-    <t>penang</t>
-  </si>
-  <si>
-    <t>perak</t>
-  </si>
-  <si>
-    <t>selangor</t>
-  </si>
-  <si>
-    <t>kl</t>
-  </si>
-  <si>
-    <t>putrajaya</t>
-  </si>
-  <si>
-    <t>ns</t>
-  </si>
-  <si>
-    <t>melaka</t>
-  </si>
-  <si>
-    <t>kelantan</t>
-  </si>
-  <si>
-    <t>terengganu</t>
-  </si>
-  <si>
-    <t>pahang</t>
-  </si>
-  <si>
-    <t>johor</t>
-  </si>
-  <si>
-    <t>sabah</t>
-  </si>
-  <si>
-    <t>labuan</t>
-  </si>
-  <si>
-    <t>sarawak</t>
+    <t>Kedah</t>
   </si>
 </sst>
 </file>
@@ -1090,139 +1036,130 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AK39"/>
+  <dimension ref="A1:AG153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AJ20" sqref="AJ20"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AE1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AF1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AG1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44258</v>
       </c>
       <c r="B2">
         <v>1598</v>
       </c>
-      <c r="C2">
-        <v>0</v>
+      <c r="C2" t="s">
+        <v>52</v>
       </c>
       <c r="D2">
-        <v>4388</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -1311,32 +1248,19 @@
       <c r="AG2">
         <v>0</v>
       </c>
-      <c r="AH2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AI2">
-        <v>10016</v>
-      </c>
-      <c r="AJ2">
-        <v>187756</v>
-      </c>
-      <c r="AK2">
-        <f>AI2/AJ2*100</f>
-        <v>5.3345831824282586</v>
-      </c>
-    </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>44289</v>
       </c>
       <c r="B3">
         <v>1896</v>
       </c>
-      <c r="C3">
-        <v>0</v>
+      <c r="C3" t="s">
+        <v>52</v>
       </c>
       <c r="D3">
-        <v>5171</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1425,32 +1349,19 @@
       <c r="AG3">
         <v>0</v>
       </c>
-      <c r="AH3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AI3">
-        <v>33449</v>
-      </c>
-      <c r="AJ3">
-        <v>1595396</v>
-      </c>
-      <c r="AK3">
-        <f t="shared" ref="AK3:AK17" si="0">AI3/AJ3*100</f>
-        <v>2.096595453417208</v>
-      </c>
-    </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>44319</v>
       </c>
       <c r="B4">
         <v>2223</v>
       </c>
-      <c r="C4">
-        <v>0</v>
+      <c r="C4" t="s">
+        <v>52</v>
       </c>
       <c r="D4">
-        <v>5306</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1539,32 +1450,19 @@
       <c r="AG4">
         <v>0</v>
       </c>
-      <c r="AH4" t="s">
-        <v>58</v>
-      </c>
-      <c r="AI4">
-        <v>35728</v>
-      </c>
-      <c r="AJ4">
-        <v>1385097</v>
-      </c>
-      <c r="AK4">
-        <f t="shared" si="0"/>
-        <v>2.5794583339650581</v>
-      </c>
-    </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>44350</v>
       </c>
       <c r="B5">
         <v>2223</v>
       </c>
-      <c r="C5">
-        <v>0</v>
+      <c r="C5" t="s">
+        <v>52</v>
       </c>
       <c r="D5">
-        <v>5414</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -1653,32 +1551,19 @@
       <c r="AG5">
         <v>0</v>
       </c>
-      <c r="AH5" t="s">
-        <v>59</v>
-      </c>
-      <c r="AI5">
-        <v>52639</v>
-      </c>
-      <c r="AJ5">
-        <v>1932525</v>
-      </c>
-      <c r="AK5">
-        <f t="shared" si="0"/>
-        <v>2.7238457458506358</v>
-      </c>
-    </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>44380</v>
       </c>
       <c r="B6">
         <v>2223</v>
       </c>
-      <c r="C6">
-        <v>0</v>
+      <c r="C6" t="s">
+        <v>52</v>
       </c>
       <c r="D6">
-        <v>6269</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1767,32 +1652,19 @@
       <c r="AG6">
         <v>0</v>
       </c>
-      <c r="AH6" t="s">
-        <v>60</v>
-      </c>
-      <c r="AI6">
-        <v>76273</v>
-      </c>
-      <c r="AJ6">
-        <v>4838547</v>
-      </c>
-      <c r="AK6">
-        <f t="shared" si="0"/>
-        <v>1.5763616639458085</v>
-      </c>
-    </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>44411</v>
       </c>
       <c r="B7">
         <v>3062</v>
       </c>
-      <c r="C7">
-        <v>0</v>
+      <c r="C7" t="s">
+        <v>52</v>
       </c>
       <c r="D7">
-        <v>9358</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1881,32 +1753,19 @@
       <c r="AG7">
         <v>0</v>
       </c>
-      <c r="AH7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AI7">
-        <v>52110</v>
-      </c>
-      <c r="AJ7">
-        <v>1481138</v>
-      </c>
-      <c r="AK7">
-        <f t="shared" si="0"/>
-        <v>3.5182407041072472</v>
-      </c>
-    </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>44442</v>
       </c>
       <c r="B8">
         <v>4158</v>
       </c>
-      <c r="C8">
-        <v>0</v>
+      <c r="C8" t="s">
+        <v>52</v>
       </c>
       <c r="D8">
-        <v>11638</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1995,32 +1854,19 @@
       <c r="AG8">
         <v>0</v>
       </c>
-      <c r="AH8" t="s">
-        <v>62</v>
-      </c>
-      <c r="AI8">
-        <v>7222</v>
-      </c>
-      <c r="AJ8">
-        <v>56913</v>
-      </c>
-      <c r="AK8">
-        <f t="shared" si="0"/>
-        <v>12.689543689490979</v>
-      </c>
-    </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>44472</v>
       </c>
       <c r="B9">
         <v>5241</v>
       </c>
-      <c r="C9">
-        <v>0</v>
+      <c r="C9" t="s">
+        <v>52</v>
       </c>
       <c r="D9">
-        <v>14200</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -2109,32 +1955,19 @@
       <c r="AG9">
         <v>0</v>
       </c>
-      <c r="AH9" t="s">
-        <v>63</v>
-      </c>
-      <c r="AI9">
-        <v>29765</v>
-      </c>
-      <c r="AJ9">
-        <v>850890</v>
-      </c>
-      <c r="AK9">
-        <f t="shared" si="0"/>
-        <v>3.4981019873309123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>44503</v>
       </c>
       <c r="B10">
         <v>6006</v>
       </c>
-      <c r="C10">
-        <v>0</v>
+      <c r="C10" t="s">
+        <v>52</v>
       </c>
       <c r="D10">
-        <v>15834</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -2223,32 +2056,19 @@
       <c r="AG10">
         <v>0</v>
       </c>
-      <c r="AH10" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI10">
-        <v>16566</v>
-      </c>
-      <c r="AJ10">
-        <v>701711</v>
-      </c>
-      <c r="AK10">
-        <f t="shared" si="0"/>
-        <v>2.360800956519137</v>
-      </c>
-    </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>44533</v>
       </c>
       <c r="B11">
         <v>6591</v>
       </c>
-      <c r="C11">
-        <v>0</v>
+      <c r="C11" t="s">
+        <v>52</v>
       </c>
       <c r="D11">
-        <v>16546</v>
+        <v>1</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -2337,32 +2157,19 @@
       <c r="AG11">
         <v>0</v>
       </c>
-      <c r="AH11" t="s">
-        <v>65</v>
-      </c>
-      <c r="AI11">
-        <v>25293</v>
-      </c>
-      <c r="AJ11">
-        <v>1237273</v>
-      </c>
-      <c r="AK11">
-        <f t="shared" si="0"/>
-        <v>2.0442537742276765</v>
-      </c>
-    </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B12">
         <v>6807</v>
       </c>
-      <c r="C12">
-        <v>0</v>
+      <c r="C12" t="s">
+        <v>52</v>
       </c>
       <c r="D12">
-        <v>17114</v>
+        <v>1</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -2451,32 +2258,19 @@
       <c r="AG12">
         <v>0</v>
       </c>
-      <c r="AH12" t="s">
-        <v>66</v>
-      </c>
-      <c r="AI12">
-        <v>26557</v>
-      </c>
-      <c r="AJ12">
-        <v>841837</v>
-      </c>
-      <c r="AK12">
-        <f t="shared" si="0"/>
-        <v>3.1546487027773789</v>
-      </c>
-    </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B13">
         <v>6807</v>
       </c>
-      <c r="C13">
-        <v>0</v>
+      <c r="C13" t="s">
+        <v>52</v>
       </c>
       <c r="D13">
-        <v>18539</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -2565,32 +2359,19 @@
       <c r="AG13">
         <v>0</v>
       </c>
-      <c r="AH13" t="s">
-        <v>67</v>
-      </c>
-      <c r="AI13">
-        <v>36049</v>
-      </c>
-      <c r="AJ13">
-        <v>1235357</v>
-      </c>
-      <c r="AK13">
-        <f t="shared" si="0"/>
-        <v>2.9181038355714182</v>
-      </c>
-    </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B14">
         <v>7276</v>
       </c>
-      <c r="C14">
-        <v>0</v>
+      <c r="C14" t="s">
+        <v>52</v>
       </c>
       <c r="D14">
-        <v>21171</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -2679,32 +2460,19 @@
       <c r="AG14">
         <v>0</v>
       </c>
-      <c r="AH14" t="s">
-        <v>68</v>
-      </c>
-      <c r="AI14">
-        <v>49401</v>
-      </c>
-      <c r="AJ14">
-        <v>2839652</v>
-      </c>
-      <c r="AK14">
-        <f t="shared" si="0"/>
-        <v>1.7396850036553775</v>
-      </c>
-    </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B15">
         <v>8038</v>
       </c>
-      <c r="C15">
-        <v>0</v>
+      <c r="C15" t="s">
+        <v>52</v>
       </c>
       <c r="D15">
-        <v>23871</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -2793,32 +2561,19 @@
       <c r="AG15">
         <v>0</v>
       </c>
-      <c r="AH15" t="s">
-        <v>69</v>
-      </c>
-      <c r="AI15">
-        <v>53859</v>
-      </c>
-      <c r="AJ15">
-        <v>2921000</v>
-      </c>
-      <c r="AK15">
-        <f t="shared" si="0"/>
-        <v>1.8438548442314275</v>
-      </c>
-    </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B16">
         <v>8795</v>
       </c>
-      <c r="C16">
-        <v>0</v>
+      <c r="C16" t="s">
+        <v>52</v>
       </c>
       <c r="D16">
-        <v>25492</v>
+        <v>1</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -2907,32 +2662,19 @@
       <c r="AG16">
         <v>0</v>
       </c>
-      <c r="AH16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AI16">
-        <v>3331</v>
-      </c>
-      <c r="AJ16">
-        <v>72272</v>
-      </c>
-      <c r="AK16">
-        <f t="shared" si="0"/>
-        <v>4.6089771972548155</v>
-      </c>
-    </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B17">
         <v>9519</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17">
         <v>1</v>
-      </c>
-      <c r="D17">
-        <v>25958</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -3021,32 +2763,19 @@
       <c r="AG17">
         <v>0</v>
       </c>
-      <c r="AH17" t="s">
-        <v>71</v>
-      </c>
-      <c r="AI17">
-        <v>57682</v>
-      </c>
-      <c r="AJ17">
-        <v>2072490</v>
-      </c>
-      <c r="AK17">
-        <f t="shared" si="0"/>
-        <v>2.7832221144613487</v>
-      </c>
-    </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B18">
         <v>9526</v>
       </c>
-      <c r="C18">
-        <v>154</v>
+      <c r="C18" t="s">
+        <v>52</v>
       </c>
       <c r="D18">
-        <v>26259</v>
+        <v>1</v>
       </c>
       <c r="E18">
         <v>6</v>
@@ -3136,18 +2865,18 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B19">
         <v>9526</v>
       </c>
-      <c r="C19">
-        <v>156</v>
+      <c r="C19" t="s">
+        <v>52</v>
       </c>
       <c r="D19">
-        <v>26265</v>
+        <v>1</v>
       </c>
       <c r="E19">
         <v>6</v>
@@ -3237,18 +2966,18 @@
         <v>4848</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B20">
         <v>9526</v>
       </c>
-      <c r="C20">
-        <v>156</v>
+      <c r="C20" t="s">
+        <v>52</v>
       </c>
       <c r="D20">
-        <v>26271</v>
+        <v>1</v>
       </c>
       <c r="E20">
         <v>719</v>
@@ -3338,18 +3067,18 @@
         <v>7735</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B21">
         <v>9526</v>
       </c>
-      <c r="C21">
-        <v>504</v>
+      <c r="C21" t="s">
+        <v>52</v>
       </c>
       <c r="D21">
-        <v>26287</v>
+        <v>1</v>
       </c>
       <c r="E21">
         <v>1896</v>
@@ -3439,18 +3168,18 @@
         <v>9537</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B22">
         <v>9526</v>
       </c>
-      <c r="C22">
-        <v>1037</v>
+      <c r="C22" t="s">
+        <v>52</v>
       </c>
       <c r="D22">
-        <v>26293</v>
+        <v>1</v>
       </c>
       <c r="E22">
         <v>3138</v>
@@ -3540,18 +3269,18 @@
         <v>10166</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B23">
         <v>9530</v>
       </c>
-      <c r="C23">
-        <v>1561</v>
+      <c r="C23" t="s">
+        <v>52</v>
       </c>
       <c r="D23">
-        <v>26310</v>
+        <v>1</v>
       </c>
       <c r="E23">
         <v>4469</v>
@@ -3641,18 +3370,18 @@
         <v>10643</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B24">
         <v>9533</v>
       </c>
-      <c r="C24">
-        <v>1853</v>
+      <c r="C24" t="s">
+        <v>52</v>
       </c>
       <c r="D24">
-        <v>26316</v>
+        <v>1</v>
       </c>
       <c r="E24">
         <v>5009</v>
@@ -3742,18 +3471,18 @@
         <v>11017</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B25">
         <v>9533</v>
       </c>
-      <c r="C25">
-        <v>2157</v>
+      <c r="C25" t="s">
+        <v>52</v>
       </c>
       <c r="D25">
-        <v>26316</v>
+        <v>1</v>
       </c>
       <c r="E25">
         <v>5144</v>
@@ -3843,18 +3572,18 @@
         <v>12100</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B26">
         <v>9533</v>
       </c>
-      <c r="C26">
-        <v>2157</v>
+      <c r="C26" t="s">
+        <v>52</v>
       </c>
       <c r="D26">
-        <v>26316</v>
+        <v>1</v>
       </c>
       <c r="E26">
         <v>5238</v>
@@ -3944,18 +3673,18 @@
         <v>15135</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B27">
         <v>9533</v>
       </c>
-      <c r="C27">
-        <v>2157</v>
+      <c r="C27" t="s">
+        <v>52</v>
       </c>
       <c r="D27">
-        <v>26355</v>
+        <v>1</v>
       </c>
       <c r="E27">
         <v>6007</v>
@@ -4045,18 +3774,18 @@
         <v>19145</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B28">
         <v>9581</v>
       </c>
-      <c r="C28">
-        <v>2978</v>
+      <c r="C28" t="s">
+        <v>52</v>
       </c>
       <c r="D28">
-        <v>27257</v>
+        <v>1</v>
       </c>
       <c r="E28">
         <v>8825</v>
@@ -4146,18 +3875,18 @@
         <v>22429</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B29">
         <v>9592</v>
       </c>
-      <c r="C29">
-        <v>4035</v>
+      <c r="C29" t="s">
+        <v>52</v>
       </c>
       <c r="D29">
-        <v>28209</v>
+        <v>1</v>
       </c>
       <c r="E29">
         <v>11139</v>
@@ -4247,18 +3976,18 @@
         <v>24535</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B30">
         <v>9840</v>
       </c>
-      <c r="C30">
-        <v>4465</v>
+      <c r="C30" t="s">
+        <v>52</v>
       </c>
       <c r="D30">
-        <v>29089</v>
+        <v>1</v>
       </c>
       <c r="E30">
         <v>13650</v>
@@ -4348,18 +4077,18 @@
         <v>25236</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>44200</v>
       </c>
       <c r="B31">
         <v>9846</v>
       </c>
-      <c r="C31">
-        <v>5610</v>
+      <c r="C31" t="s">
+        <v>52</v>
       </c>
       <c r="D31">
-        <v>30316</v>
+        <v>1</v>
       </c>
       <c r="E31">
         <v>15300</v>
@@ -4449,18 +4178,18 @@
         <v>25287</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>44231</v>
       </c>
       <c r="B32">
         <v>9855</v>
       </c>
-      <c r="C32">
-        <v>6455</v>
+      <c r="C32" t="s">
+        <v>52</v>
       </c>
       <c r="D32">
-        <v>30536</v>
+        <v>1</v>
       </c>
       <c r="E32">
         <v>15698</v>
@@ -4557,11 +4286,11 @@
       <c r="B33">
         <v>9858</v>
       </c>
-      <c r="C33">
-        <v>6668</v>
+      <c r="C33" t="s">
+        <v>52</v>
       </c>
       <c r="D33">
-        <v>30550</v>
+        <v>1</v>
       </c>
       <c r="E33">
         <v>16130</v>
@@ -4658,11 +4387,11 @@
       <c r="B34">
         <v>9858</v>
       </c>
-      <c r="C34">
-        <v>6668</v>
+      <c r="C34" t="s">
+        <v>52</v>
       </c>
       <c r="D34">
-        <v>31115</v>
+        <v>1</v>
       </c>
       <c r="E34">
         <v>17493</v>
@@ -4759,11 +4488,11 @@
       <c r="B35">
         <v>9863</v>
       </c>
-      <c r="C35">
-        <v>6820</v>
+      <c r="C35" t="s">
+        <v>52</v>
       </c>
       <c r="D35">
-        <v>31324</v>
+        <v>1</v>
       </c>
       <c r="E35">
         <v>19925</v>
@@ -4860,11 +4589,11 @@
       <c r="B36">
         <v>10001</v>
       </c>
-      <c r="C36">
-        <v>6854</v>
+      <c r="C36" t="s">
+        <v>52</v>
       </c>
       <c r="D36">
-        <v>32089</v>
+        <v>1</v>
       </c>
       <c r="E36">
         <v>22579</v>
@@ -4961,11 +4690,11 @@
       <c r="B37">
         <v>10001</v>
       </c>
-      <c r="C37">
-        <v>6884</v>
+      <c r="C37" t="s">
+        <v>52</v>
       </c>
       <c r="D37">
-        <v>32556</v>
+        <v>1</v>
       </c>
       <c r="E37">
         <v>24046</v>
@@ -5062,11 +4791,11 @@
       <c r="B38">
         <v>10001</v>
       </c>
-      <c r="C38">
-        <v>6920</v>
+      <c r="C38" t="s">
+        <v>52</v>
       </c>
       <c r="D38">
-        <v>32836</v>
+        <v>1</v>
       </c>
       <c r="E38">
         <v>24621</v>
@@ -5163,11 +4892,11 @@
       <c r="B39">
         <v>10016</v>
       </c>
-      <c r="C39">
-        <v>8026</v>
+      <c r="C39" t="s">
+        <v>52</v>
       </c>
       <c r="D39">
-        <v>33449</v>
+        <v>1</v>
       </c>
       <c r="E39">
         <v>24698</v>
@@ -5255,6 +4984,1374 @@
       </c>
       <c r="AG39">
         <v>30014</v>
+      </c>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>44258</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>44289</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41" t="s">
+        <v>52</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>44319</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42" t="s">
+        <v>52</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>44350</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43" t="s">
+        <v>52</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>44380</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
+        <v>44411</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45" t="s">
+        <v>52</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
+        <v>44442</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46" t="s">
+        <v>52</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
+        <v>44472</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47" t="s">
+        <v>52</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
+        <v>44503</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48" t="s">
+        <v>52</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
+        <v>44533</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49" t="s">
+        <v>52</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>30</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50" t="s">
+        <v>52</v>
+      </c>
+      <c r="D50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>31</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51" t="s">
+        <v>52</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>32</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+      <c r="C52" t="s">
+        <v>52</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>33</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53" t="s">
+        <v>52</v>
+      </c>
+      <c r="D53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>34</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54" t="s">
+        <v>52</v>
+      </c>
+      <c r="D54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>35</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>52</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>36</v>
+      </c>
+      <c r="B56">
+        <v>154</v>
+      </c>
+      <c r="C56" t="s">
+        <v>52</v>
+      </c>
+      <c r="D56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>37</v>
+      </c>
+      <c r="B57">
+        <v>156</v>
+      </c>
+      <c r="C57" t="s">
+        <v>52</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>38</v>
+      </c>
+      <c r="B58">
+        <v>156</v>
+      </c>
+      <c r="C58" t="s">
+        <v>52</v>
+      </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>39</v>
+      </c>
+      <c r="B59">
+        <v>504</v>
+      </c>
+      <c r="C59" t="s">
+        <v>52</v>
+      </c>
+      <c r="D59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>40</v>
+      </c>
+      <c r="B60">
+        <v>1037</v>
+      </c>
+      <c r="C60" t="s">
+        <v>52</v>
+      </c>
+      <c r="D60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>41</v>
+      </c>
+      <c r="B61">
+        <v>1561</v>
+      </c>
+      <c r="C61" t="s">
+        <v>52</v>
+      </c>
+      <c r="D61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>42</v>
+      </c>
+      <c r="B62">
+        <v>1853</v>
+      </c>
+      <c r="C62" t="s">
+        <v>52</v>
+      </c>
+      <c r="D62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>43</v>
+      </c>
+      <c r="B63">
+        <v>2157</v>
+      </c>
+      <c r="C63" t="s">
+        <v>52</v>
+      </c>
+      <c r="D63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>44</v>
+      </c>
+      <c r="B64">
+        <v>2157</v>
+      </c>
+      <c r="C64" t="s">
+        <v>52</v>
+      </c>
+      <c r="D64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>45</v>
+      </c>
+      <c r="B65">
+        <v>2157</v>
+      </c>
+      <c r="C65" t="s">
+        <v>52</v>
+      </c>
+      <c r="D65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>46</v>
+      </c>
+      <c r="B66">
+        <v>2978</v>
+      </c>
+      <c r="C66" t="s">
+        <v>52</v>
+      </c>
+      <c r="D66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>47</v>
+      </c>
+      <c r="B67">
+        <v>4035</v>
+      </c>
+      <c r="C67" t="s">
+        <v>52</v>
+      </c>
+      <c r="D67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>48</v>
+      </c>
+      <c r="B68">
+        <v>4465</v>
+      </c>
+      <c r="C68" t="s">
+        <v>52</v>
+      </c>
+      <c r="D68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="1">
+        <v>44200</v>
+      </c>
+      <c r="B69">
+        <v>5610</v>
+      </c>
+      <c r="C69" t="s">
+        <v>52</v>
+      </c>
+      <c r="D69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="1">
+        <v>44231</v>
+      </c>
+      <c r="B70">
+        <v>6455</v>
+      </c>
+      <c r="C70" t="s">
+        <v>52</v>
+      </c>
+      <c r="D70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="1">
+        <v>44259</v>
+      </c>
+      <c r="B71">
+        <v>6668</v>
+      </c>
+      <c r="C71" t="s">
+        <v>52</v>
+      </c>
+      <c r="D71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="1">
+        <v>44290</v>
+      </c>
+      <c r="B72">
+        <v>6668</v>
+      </c>
+      <c r="C72" t="s">
+        <v>52</v>
+      </c>
+      <c r="D72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="1">
+        <v>44320</v>
+      </c>
+      <c r="B73">
+        <v>6820</v>
+      </c>
+      <c r="C73" t="s">
+        <v>52</v>
+      </c>
+      <c r="D73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="1">
+        <v>44351</v>
+      </c>
+      <c r="B74">
+        <v>6854</v>
+      </c>
+      <c r="C74" t="s">
+        <v>52</v>
+      </c>
+      <c r="D74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="1">
+        <v>44381</v>
+      </c>
+      <c r="B75">
+        <v>6884</v>
+      </c>
+      <c r="C75" t="s">
+        <v>52</v>
+      </c>
+      <c r="D75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="1">
+        <v>44412</v>
+      </c>
+      <c r="B76">
+        <v>6920</v>
+      </c>
+      <c r="C76" t="s">
+        <v>52</v>
+      </c>
+      <c r="D76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="1">
+        <v>44443</v>
+      </c>
+      <c r="B77">
+        <v>8026</v>
+      </c>
+      <c r="C77" t="s">
+        <v>52</v>
+      </c>
+      <c r="D77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="1">
+        <v>44258</v>
+      </c>
+      <c r="B78">
+        <v>4388</v>
+      </c>
+      <c r="C78" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="1">
+        <v>44289</v>
+      </c>
+      <c r="B79">
+        <v>5171</v>
+      </c>
+      <c r="C79" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="1">
+        <v>44319</v>
+      </c>
+      <c r="B80">
+        <v>5306</v>
+      </c>
+      <c r="C80" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="1">
+        <v>44350</v>
+      </c>
+      <c r="B81">
+        <v>5414</v>
+      </c>
+      <c r="C81" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="1">
+        <v>44380</v>
+      </c>
+      <c r="B82">
+        <v>6269</v>
+      </c>
+      <c r="C82" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="1">
+        <v>44411</v>
+      </c>
+      <c r="B83">
+        <v>9358</v>
+      </c>
+      <c r="C83" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="1">
+        <v>44442</v>
+      </c>
+      <c r="B84">
+        <v>11638</v>
+      </c>
+      <c r="C84" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="1">
+        <v>44472</v>
+      </c>
+      <c r="B85">
+        <v>14200</v>
+      </c>
+      <c r="C85" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="1">
+        <v>44503</v>
+      </c>
+      <c r="B86">
+        <v>15834</v>
+      </c>
+      <c r="C86" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="1">
+        <v>44533</v>
+      </c>
+      <c r="B87">
+        <v>16546</v>
+      </c>
+      <c r="C87" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>30</v>
+      </c>
+      <c r="B88">
+        <v>17114</v>
+      </c>
+      <c r="C88" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>31</v>
+      </c>
+      <c r="B89">
+        <v>18539</v>
+      </c>
+      <c r="C89" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>32</v>
+      </c>
+      <c r="B90">
+        <v>21171</v>
+      </c>
+      <c r="C90" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>33</v>
+      </c>
+      <c r="B91">
+        <v>23871</v>
+      </c>
+      <c r="C91" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>34</v>
+      </c>
+      <c r="B92">
+        <v>25492</v>
+      </c>
+      <c r="C92" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>35</v>
+      </c>
+      <c r="B93">
+        <v>25958</v>
+      </c>
+      <c r="C93" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>36</v>
+      </c>
+      <c r="B94">
+        <v>26259</v>
+      </c>
+      <c r="C94" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>37</v>
+      </c>
+      <c r="B95">
+        <v>26265</v>
+      </c>
+      <c r="C95" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>38</v>
+      </c>
+      <c r="B96">
+        <v>26271</v>
+      </c>
+      <c r="C96" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>39</v>
+      </c>
+      <c r="B97">
+        <v>26287</v>
+      </c>
+      <c r="C97" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>40</v>
+      </c>
+      <c r="B98">
+        <v>26293</v>
+      </c>
+      <c r="C98" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>41</v>
+      </c>
+      <c r="B99">
+        <v>26310</v>
+      </c>
+      <c r="C99" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>42</v>
+      </c>
+      <c r="B100">
+        <v>26316</v>
+      </c>
+      <c r="C100" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>43</v>
+      </c>
+      <c r="B101">
+        <v>26316</v>
+      </c>
+      <c r="C101" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>44</v>
+      </c>
+      <c r="B102">
+        <v>26316</v>
+      </c>
+      <c r="C102" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>45</v>
+      </c>
+      <c r="B103">
+        <v>26355</v>
+      </c>
+      <c r="C103" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>46</v>
+      </c>
+      <c r="B104">
+        <v>27257</v>
+      </c>
+      <c r="C104" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>47</v>
+      </c>
+      <c r="B105">
+        <v>28209</v>
+      </c>
+      <c r="C105" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>48</v>
+      </c>
+      <c r="B106">
+        <v>29089</v>
+      </c>
+      <c r="C106" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A107" s="1">
+        <v>44200</v>
+      </c>
+      <c r="B107">
+        <v>30316</v>
+      </c>
+      <c r="C107" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A108" s="1">
+        <v>44231</v>
+      </c>
+      <c r="B108">
+        <v>30536</v>
+      </c>
+      <c r="C108" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A109" s="1">
+        <v>44259</v>
+      </c>
+      <c r="B109">
+        <v>30550</v>
+      </c>
+      <c r="C109" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A110" s="1">
+        <v>44290</v>
+      </c>
+      <c r="B110">
+        <v>31115</v>
+      </c>
+      <c r="C110" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" s="1">
+        <v>44320</v>
+      </c>
+      <c r="B111">
+        <v>31324</v>
+      </c>
+      <c r="C111" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" s="1">
+        <v>44351</v>
+      </c>
+      <c r="B112">
+        <v>32089</v>
+      </c>
+      <c r="C112" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" s="1">
+        <v>44381</v>
+      </c>
+      <c r="B113">
+        <v>32556</v>
+      </c>
+      <c r="C113" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" s="1">
+        <v>44412</v>
+      </c>
+      <c r="B114">
+        <v>32836</v>
+      </c>
+      <c r="C114" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" s="1">
+        <v>44443</v>
+      </c>
+      <c r="B115">
+        <v>33449</v>
+      </c>
+      <c r="C115" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" s="1">
+        <v>44258</v>
+      </c>
+      <c r="B116">
+        <v>4388</v>
+      </c>
+      <c r="C116" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" s="1">
+        <v>44289</v>
+      </c>
+      <c r="B117">
+        <v>5171</v>
+      </c>
+      <c r="C117" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" s="1">
+        <v>44319</v>
+      </c>
+      <c r="B118">
+        <v>5306</v>
+      </c>
+      <c r="C118" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" s="1">
+        <v>44350</v>
+      </c>
+      <c r="B119">
+        <v>5414</v>
+      </c>
+      <c r="C119" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" s="1">
+        <v>44380</v>
+      </c>
+      <c r="B120">
+        <v>6269</v>
+      </c>
+      <c r="C120" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" s="1">
+        <v>44411</v>
+      </c>
+      <c r="B121">
+        <v>9358</v>
+      </c>
+      <c r="C121" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" s="1">
+        <v>44442</v>
+      </c>
+      <c r="B122">
+        <v>11638</v>
+      </c>
+      <c r="C122" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123" s="1">
+        <v>44472</v>
+      </c>
+      <c r="B123">
+        <v>14200</v>
+      </c>
+      <c r="C123" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A124" s="1">
+        <v>44503</v>
+      </c>
+      <c r="B124">
+        <v>15834</v>
+      </c>
+      <c r="C124" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A125" s="1">
+        <v>44533</v>
+      </c>
+      <c r="B125">
+        <v>16546</v>
+      </c>
+      <c r="C125" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>30</v>
+      </c>
+      <c r="B126">
+        <v>17114</v>
+      </c>
+      <c r="C126" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>31</v>
+      </c>
+      <c r="B127">
+        <v>18539</v>
+      </c>
+      <c r="C127" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>32</v>
+      </c>
+      <c r="B128">
+        <v>21171</v>
+      </c>
+      <c r="C128" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>33</v>
+      </c>
+      <c r="B129">
+        <v>23871</v>
+      </c>
+      <c r="C129" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>34</v>
+      </c>
+      <c r="B130">
+        <v>25492</v>
+      </c>
+      <c r="C130" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>35</v>
+      </c>
+      <c r="B131">
+        <v>25958</v>
+      </c>
+      <c r="C131" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>36</v>
+      </c>
+      <c r="B132">
+        <v>26259</v>
+      </c>
+      <c r="C132" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>37</v>
+      </c>
+      <c r="B133">
+        <v>26265</v>
+      </c>
+      <c r="C133" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>38</v>
+      </c>
+      <c r="B134">
+        <v>26271</v>
+      </c>
+      <c r="C134" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>39</v>
+      </c>
+      <c r="B135">
+        <v>26287</v>
+      </c>
+      <c r="C135" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>40</v>
+      </c>
+      <c r="B136">
+        <v>26293</v>
+      </c>
+      <c r="C136" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>41</v>
+      </c>
+      <c r="B137">
+        <v>26310</v>
+      </c>
+      <c r="C137" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>42</v>
+      </c>
+      <c r="B138">
+        <v>26316</v>
+      </c>
+      <c r="C138" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>43</v>
+      </c>
+      <c r="B139">
+        <v>26316</v>
+      </c>
+      <c r="C139" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>44</v>
+      </c>
+      <c r="B140">
+        <v>26316</v>
+      </c>
+      <c r="C140" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>45</v>
+      </c>
+      <c r="B141">
+        <v>26355</v>
+      </c>
+      <c r="C141" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>46</v>
+      </c>
+      <c r="B142">
+        <v>27257</v>
+      </c>
+      <c r="C142" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>47</v>
+      </c>
+      <c r="B143">
+        <v>28209</v>
+      </c>
+      <c r="C143" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>48</v>
+      </c>
+      <c r="B144">
+        <v>29089</v>
+      </c>
+      <c r="C144" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A145" s="1">
+        <v>44200</v>
+      </c>
+      <c r="B145">
+        <v>30316</v>
+      </c>
+      <c r="C145" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A146" s="1">
+        <v>44231</v>
+      </c>
+      <c r="B146">
+        <v>30536</v>
+      </c>
+      <c r="C146" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A147" s="1">
+        <v>44259</v>
+      </c>
+      <c r="B147">
+        <v>30550</v>
+      </c>
+      <c r="C147" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A148" s="1">
+        <v>44290</v>
+      </c>
+      <c r="B148">
+        <v>31115</v>
+      </c>
+      <c r="C148" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A149" s="1">
+        <v>44320</v>
+      </c>
+      <c r="B149">
+        <v>31324</v>
+      </c>
+      <c r="C149" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A150" s="1">
+        <v>44351</v>
+      </c>
+      <c r="B150">
+        <v>32089</v>
+      </c>
+      <c r="C150" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A151" s="1">
+        <v>44381</v>
+      </c>
+      <c r="B151">
+        <v>32556</v>
+      </c>
+      <c r="C151" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A152" s="1">
+        <v>44412</v>
+      </c>
+      <c r="B152">
+        <v>32836</v>
+      </c>
+      <c r="C152" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A153" s="1">
+        <v>44443</v>
+      </c>
+      <c r="B153">
+        <v>33449</v>
+      </c>
+      <c r="C153" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>